<commit_message>
[Feat] NPC 대화 조정
</commit_message>
<xml_diff>
--- a/Assets/02.Scripts/12.NPC/TextUIManager/BlackSmith.xlsx
+++ b/Assets/02.Scripts/12.NPC/TextUIManager/BlackSmith.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unity\Become_Celebrity_on_Farm\Assets\02.Scripts\12.NPC\TextUIManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5D26B6-9ADA-4D8A-8B32-63A0D5BA4A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A583C5B-A3C3-4300-B8DD-5D75D4D7C7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="945" windowWidth="12870" windowHeight="13755" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,6 @@
     <t>BlackSmith_0</t>
   </si>
   <si>
-    <t>실험용 1회용 대사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘 날씨는 어때</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>BlackSmith_3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -57,7 +49,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>반복용 대사 없는거 빼곤 다 있다고</t>
+    <t>오늘도 왔는가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>요즘 농사는 괜찮게 되고 있지?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리 마을의 유일 마트라고</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -384,7 +384,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -395,7 +395,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -407,10 +407,10 @@
         <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G1" t="b">
         <v>1</v>
@@ -418,7 +418,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -430,10 +430,10 @@
         <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -441,10 +441,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -453,10 +453,10 @@
         <v>100</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -476,10 +476,10 @@
         <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>

</xml_diff>